<commit_message>
Changed JLCPCB to JLCPCB PN
Also fixed up the positions of some of the symbols.
</commit_message>
<xml_diff>
--- a/symbols/!Capacitor-0603.xlsx
+++ b/symbols/!Capacitor-0603.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbwal\VSCode\KiCAD\electronics-library\symbols\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A84BA54-244F-4181-B20F-7196CD345373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ED2D6E-978E-478E-B0DE-A0A64302021B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32160" yWindow="1200" windowWidth="21600" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52365" yWindow="1320" windowWidth="22740" windowHeight="17595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="~Template" sheetId="1" r:id="rId1"/>
@@ -377,9 +377,6 @@
     <t>6.3V</t>
   </si>
   <si>
-    <t>JLCPCB</t>
-  </si>
-  <si>
     <t>C1588</t>
   </si>
   <si>
@@ -687,6 +684,9 @@
   </si>
   <si>
     <t>8.2nF 50V X7R ±10%</t>
+  </si>
+  <si>
+    <t>JLCPCB PN</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1029,7 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A48"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,10 +1051,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>213</v>
       </c>
       <c r="C1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -1066,7 +1066,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -1084,13 +1084,13 @@
         <v>1nF_X7R_50V</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E2" t="s">
         <v>54</v>
@@ -1099,7 +1099,7 @@
         <v>105</v>
       </c>
       <c r="G2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
@@ -1108,7 +1108,7 @@
         <v>101</v>
       </c>
       <c r="J2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1117,13 +1117,13 @@
         <v>150pF_X7R_50V</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E3" t="s">
         <v>55</v>
@@ -1132,7 +1132,7 @@
         <v>105</v>
       </c>
       <c r="G3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
@@ -1141,7 +1141,7 @@
         <v>101</v>
       </c>
       <c r="J3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1150,13 +1150,13 @@
         <v>1.5nF_X7R_50V</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
@@ -1165,7 +1165,7 @@
         <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H4" t="s">
         <v>9</v>
@@ -1174,7 +1174,7 @@
         <v>101</v>
       </c>
       <c r="J4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1183,13 +1183,13 @@
         <v>15nF_X7R_50V</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E5" t="s">
         <v>57</v>
@@ -1198,7 +1198,7 @@
         <v>105</v>
       </c>
       <c r="G5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -1207,7 +1207,7 @@
         <v>101</v>
       </c>
       <c r="J5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1216,13 +1216,13 @@
         <v>200pF_X7R_50V</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E6" t="s">
         <v>58</v>
@@ -1231,7 +1231,7 @@
         <v>105</v>
       </c>
       <c r="G6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
@@ -1240,7 +1240,7 @@
         <v>101</v>
       </c>
       <c r="J6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1249,13 +1249,13 @@
         <v>220pF_X7R_50V</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E7" t="s">
         <v>59</v>
@@ -1264,7 +1264,7 @@
         <v>105</v>
       </c>
       <c r="G7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
@@ -1273,7 +1273,7 @@
         <v>101</v>
       </c>
       <c r="J7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1282,13 +1282,13 @@
         <v>2.2nF_X7R_50V</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E8" t="s">
         <v>60</v>
@@ -1297,7 +1297,7 @@
         <v>105</v>
       </c>
       <c r="G8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H8" t="s">
         <v>13</v>
@@ -1306,7 +1306,7 @@
         <v>101</v>
       </c>
       <c r="J8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1315,13 +1315,13 @@
         <v>2.7nF_X7R_50V</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E9" t="s">
         <v>61</v>
@@ -1330,7 +1330,7 @@
         <v>105</v>
       </c>
       <c r="G9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
@@ -1339,7 +1339,7 @@
         <v>101</v>
       </c>
       <c r="J9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1348,13 +1348,13 @@
         <v>3.3nF_X7R_50V</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E10" t="s">
         <v>62</v>
@@ -1363,7 +1363,7 @@
         <v>105</v>
       </c>
       <c r="G10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -1372,7 +1372,7 @@
         <v>101</v>
       </c>
       <c r="J10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1381,13 +1381,13 @@
         <v>330nF_X7R_25V</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E11" t="s">
         <v>63</v>
@@ -1396,7 +1396,7 @@
         <v>106</v>
       </c>
       <c r="G11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H11" t="s">
         <v>16</v>
@@ -1405,7 +1405,7 @@
         <v>101</v>
       </c>
       <c r="J11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1414,13 +1414,13 @@
         <v>470pF_X7R_50V</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E12" t="s">
         <v>64</v>
@@ -1429,7 +1429,7 @@
         <v>105</v>
       </c>
       <c r="G12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H12" t="s">
         <v>17</v>
@@ -1438,7 +1438,7 @@
         <v>101</v>
       </c>
       <c r="J12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1447,13 +1447,13 @@
         <v>47nF_X7R_50V</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" t="s">
         <v>65</v>
@@ -1462,7 +1462,7 @@
         <v>105</v>
       </c>
       <c r="G13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H13" t="s">
         <v>18</v>
@@ -1471,7 +1471,7 @@
         <v>101</v>
       </c>
       <c r="J13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1480,13 +1480,13 @@
         <v>470nF_X7R_25V</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E14" t="s">
         <v>66</v>
@@ -1495,7 +1495,7 @@
         <v>106</v>
       </c>
       <c r="G14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -1504,7 +1504,7 @@
         <v>101</v>
       </c>
       <c r="J14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1513,13 +1513,13 @@
         <v>680pF_X7R_50V</v>
       </c>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E15" t="s">
         <v>67</v>
@@ -1528,7 +1528,7 @@
         <v>105</v>
       </c>
       <c r="G15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H15" t="s">
         <v>20</v>
@@ -1537,7 +1537,7 @@
         <v>101</v>
       </c>
       <c r="J15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1546,13 +1546,13 @@
         <v>6.8nF_X7R_50V</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E16" t="s">
         <v>68</v>
@@ -1561,7 +1561,7 @@
         <v>105</v>
       </c>
       <c r="G16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H16" t="s">
         <v>21</v>
@@ -1570,7 +1570,7 @@
         <v>101</v>
       </c>
       <c r="J16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1579,13 +1579,13 @@
         <v>10pF_C0G_50V</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E17" t="s">
         <v>69</v>
@@ -1594,7 +1594,7 @@
         <v>105</v>
       </c>
       <c r="G17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H17" t="s">
         <v>22</v>
@@ -1603,7 +1603,7 @@
         <v>102</v>
       </c>
       <c r="J17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1612,13 +1612,13 @@
         <v>15pF_C0G_50V</v>
       </c>
       <c r="B18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E18" t="s">
         <v>70</v>
@@ -1627,7 +1627,7 @@
         <v>105</v>
       </c>
       <c r="G18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H18" t="s">
         <v>23</v>
@@ -1636,7 +1636,7 @@
         <v>102</v>
       </c>
       <c r="J18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1645,13 +1645,13 @@
         <v>18pF_C0G_50V</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E19" t="s">
         <v>71</v>
@@ -1660,7 +1660,7 @@
         <v>105</v>
       </c>
       <c r="G19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H19" t="s">
         <v>24</v>
@@ -1669,7 +1669,7 @@
         <v>102</v>
       </c>
       <c r="J19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1678,13 +1678,13 @@
         <v>20pF_C0G_50V</v>
       </c>
       <c r="B20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E20" t="s">
         <v>72</v>
@@ -1693,7 +1693,7 @@
         <v>105</v>
       </c>
       <c r="G20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H20" t="s">
         <v>25</v>
@@ -1702,7 +1702,7 @@
         <v>102</v>
       </c>
       <c r="J20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1711,13 +1711,13 @@
         <v>22pF_C0G_50V</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E21" t="s">
         <v>73</v>
@@ -1726,7 +1726,7 @@
         <v>105</v>
       </c>
       <c r="G21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H21" t="s">
         <v>26</v>
@@ -1735,7 +1735,7 @@
         <v>102</v>
       </c>
       <c r="J21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1744,13 +1744,13 @@
         <v>30pF_C0G_50V</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E22" t="s">
         <v>74</v>
@@ -1759,7 +1759,7 @@
         <v>105</v>
       </c>
       <c r="G22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H22" t="s">
         <v>27</v>
@@ -1768,7 +1768,7 @@
         <v>102</v>
       </c>
       <c r="J22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1777,13 +1777,13 @@
         <v>33pF_C0G_50V</v>
       </c>
       <c r="B23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E23" t="s">
         <v>75</v>
@@ -1792,7 +1792,7 @@
         <v>105</v>
       </c>
       <c r="G23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H23" t="s">
         <v>28</v>
@@ -1801,7 +1801,7 @@
         <v>102</v>
       </c>
       <c r="J23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1810,13 +1810,13 @@
         <v>330pF_C0G_50V</v>
       </c>
       <c r="B24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E24" t="s">
         <v>76</v>
@@ -1825,7 +1825,7 @@
         <v>105</v>
       </c>
       <c r="G24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H24" t="s">
         <v>29</v>
@@ -1834,7 +1834,7 @@
         <v>102</v>
       </c>
       <c r="J24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1843,13 +1843,13 @@
         <v>4.7pF_C0G_50V</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E25" t="s">
         <v>77</v>
@@ -1858,7 +1858,7 @@
         <v>105</v>
       </c>
       <c r="G25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H25" t="s">
         <v>30</v>
@@ -1867,7 +1867,7 @@
         <v>102</v>
       </c>
       <c r="J25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1876,13 +1876,13 @@
         <v>47pF_C0G_50V</v>
       </c>
       <c r="B26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E26" t="s">
         <v>78</v>
@@ -1891,7 +1891,7 @@
         <v>105</v>
       </c>
       <c r="G26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H26" t="s">
         <v>31</v>
@@ -1900,7 +1900,7 @@
         <v>102</v>
       </c>
       <c r="J26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1909,13 +1909,13 @@
         <v>6.8pF_C0G_50V</v>
       </c>
       <c r="B27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E27" t="s">
         <v>79</v>
@@ -1924,7 +1924,7 @@
         <v>105</v>
       </c>
       <c r="G27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H27" t="s">
         <v>32</v>
@@ -1933,7 +1933,7 @@
         <v>102</v>
       </c>
       <c r="J27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1942,13 +1942,13 @@
         <v>8.2pF_C0G_50V</v>
       </c>
       <c r="B28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E28" t="s">
         <v>80</v>
@@ -1957,7 +1957,7 @@
         <v>105</v>
       </c>
       <c r="G28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H28" t="s">
         <v>33</v>
@@ -1966,7 +1966,7 @@
         <v>102</v>
       </c>
       <c r="J28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1975,13 +1975,13 @@
         <v>100nF_X7R_50V</v>
       </c>
       <c r="B29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E29" t="s">
         <v>81</v>
@@ -1990,7 +1990,7 @@
         <v>105</v>
       </c>
       <c r="G29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H29" t="s">
         <v>34</v>
@@ -1999,7 +1999,7 @@
         <v>101</v>
       </c>
       <c r="J29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2008,13 +2008,13 @@
         <v>100pF_C0G_50V</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E30" t="s">
         <v>82</v>
@@ -2023,7 +2023,7 @@
         <v>105</v>
       </c>
       <c r="G30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H30" t="s">
         <v>35</v>
@@ -2032,7 +2032,7 @@
         <v>102</v>
       </c>
       <c r="J30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2041,13 +2041,13 @@
         <v>1uF_X5R_50V</v>
       </c>
       <c r="B31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E31" t="s">
         <v>83</v>
@@ -2056,7 +2056,7 @@
         <v>105</v>
       </c>
       <c r="G31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H31" t="s">
         <v>36</v>
@@ -2065,7 +2065,7 @@
         <v>103</v>
       </c>
       <c r="J31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2074,13 +2074,13 @@
         <v>4.7uF_X5R_16V</v>
       </c>
       <c r="B32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E32" t="s">
         <v>84</v>
@@ -2089,7 +2089,7 @@
         <v>107</v>
       </c>
       <c r="G32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H32" t="s">
         <v>37</v>
@@ -2098,7 +2098,7 @@
         <v>103</v>
       </c>
       <c r="J32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2107,13 +2107,13 @@
         <v>10uF_X5R_10V</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E33" t="s">
         <v>85</v>
@@ -2122,7 +2122,7 @@
         <v>108</v>
       </c>
       <c r="G33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H33" t="s">
         <v>38</v>
@@ -2131,7 +2131,7 @@
         <v>103</v>
       </c>
       <c r="J33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2140,13 +2140,13 @@
         <v>33nF_X7R_50V</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E34" t="s">
         <v>86</v>
@@ -2155,7 +2155,7 @@
         <v>105</v>
       </c>
       <c r="G34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H34" t="s">
         <v>39</v>
@@ -2164,7 +2164,7 @@
         <v>101</v>
       </c>
       <c r="J34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2173,13 +2173,13 @@
         <v>220nF_X7R_25V</v>
       </c>
       <c r="B35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E35" t="s">
         <v>87</v>
@@ -2188,7 +2188,7 @@
         <v>106</v>
       </c>
       <c r="G35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H35" t="s">
         <v>40</v>
@@ -2197,7 +2197,7 @@
         <v>101</v>
       </c>
       <c r="J35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2206,13 +2206,13 @@
         <v>22nF_X7R_50V</v>
       </c>
       <c r="B36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E36" t="s">
         <v>88</v>
@@ -2221,7 +2221,7 @@
         <v>105</v>
       </c>
       <c r="G36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H36" t="s">
         <v>41</v>
@@ -2230,7 +2230,7 @@
         <v>101</v>
       </c>
       <c r="J36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2239,13 +2239,13 @@
         <v>2.2uF_X5R_16V</v>
       </c>
       <c r="B37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E37" t="s">
         <v>89</v>
@@ -2254,7 +2254,7 @@
         <v>107</v>
       </c>
       <c r="G37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H37" t="s">
         <v>42</v>
@@ -2263,7 +2263,7 @@
         <v>103</v>
       </c>
       <c r="J37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2272,13 +2272,13 @@
         <v>68pF_C0G_50V</v>
       </c>
       <c r="B38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E38" t="s">
         <v>90</v>
@@ -2287,7 +2287,7 @@
         <v>105</v>
       </c>
       <c r="G38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H38" t="s">
         <v>43</v>
@@ -2296,7 +2296,7 @@
         <v>102</v>
       </c>
       <c r="J38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2305,13 +2305,13 @@
         <v>68nF_X7R_50V</v>
       </c>
       <c r="B39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E39" t="s">
         <v>91</v>
@@ -2320,7 +2320,7 @@
         <v>105</v>
       </c>
       <c r="G39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H39" t="s">
         <v>44</v>
@@ -2329,7 +2329,7 @@
         <v>101</v>
       </c>
       <c r="J39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2338,13 +2338,13 @@
         <v>6pF_C0G_50V</v>
       </c>
       <c r="B40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E40" t="s">
         <v>92</v>
@@ -2353,7 +2353,7 @@
         <v>105</v>
       </c>
       <c r="G40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H40" t="s">
         <v>45</v>
@@ -2362,7 +2362,7 @@
         <v>102</v>
       </c>
       <c r="J40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2371,13 +2371,13 @@
         <v>12pF_C0G_50V</v>
       </c>
       <c r="B41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E41" t="s">
         <v>93</v>
@@ -2386,7 +2386,7 @@
         <v>105</v>
       </c>
       <c r="G41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H41" t="s">
         <v>46</v>
@@ -2395,7 +2395,7 @@
         <v>102</v>
       </c>
       <c r="J41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2404,13 +2404,13 @@
         <v>56pF_C0G_50V</v>
       </c>
       <c r="B42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E42" t="s">
         <v>94</v>
@@ -2419,7 +2419,7 @@
         <v>105</v>
       </c>
       <c r="G42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H42" t="s">
         <v>47</v>
@@ -2428,7 +2428,7 @@
         <v>102</v>
       </c>
       <c r="J42" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2437,13 +2437,13 @@
         <v>3pF_C0G_50V</v>
       </c>
       <c r="B43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E43" t="s">
         <v>95</v>
@@ -2452,7 +2452,7 @@
         <v>105</v>
       </c>
       <c r="G43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H43" t="s">
         <v>48</v>
@@ -2461,7 +2461,7 @@
         <v>102</v>
       </c>
       <c r="J43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2470,13 +2470,13 @@
         <v>4.7nF_X7R_50V</v>
       </c>
       <c r="B44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D44" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E44" t="s">
         <v>96</v>
@@ -2485,7 +2485,7 @@
         <v>105</v>
       </c>
       <c r="G44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H44" t="s">
         <v>49</v>
@@ -2494,7 +2494,7 @@
         <v>101</v>
       </c>
       <c r="J44" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2503,13 +2503,13 @@
         <v>10nF_X7R_50V</v>
       </c>
       <c r="B45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D45" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E45" t="s">
         <v>97</v>
@@ -2518,7 +2518,7 @@
         <v>105</v>
       </c>
       <c r="G45" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H45" t="s">
         <v>50</v>
@@ -2527,7 +2527,7 @@
         <v>101</v>
       </c>
       <c r="J45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2536,13 +2536,13 @@
         <v>22uF_X5R_6.3V</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E46" t="s">
         <v>98</v>
@@ -2551,7 +2551,7 @@
         <v>109</v>
       </c>
       <c r="G46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H46" t="s">
         <v>51</v>
@@ -2560,7 +2560,7 @@
         <v>103</v>
       </c>
       <c r="J46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2569,13 +2569,13 @@
         <v>27pF_NP0_50V</v>
       </c>
       <c r="B47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E47" t="s">
         <v>99</v>
@@ -2584,7 +2584,7 @@
         <v>105</v>
       </c>
       <c r="G47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H47" t="s">
         <v>52</v>
@@ -2593,7 +2593,7 @@
         <v>104</v>
       </c>
       <c r="J47" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2602,13 +2602,13 @@
         <v>8.2nF_X7R_50V</v>
       </c>
       <c r="B48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D48" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E48" t="s">
         <v>100</v>
@@ -2617,7 +2617,7 @@
         <v>105</v>
       </c>
       <c r="G48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H48" t="s">
         <v>53</v>
@@ -2626,11 +2626,12 @@
         <v>101</v>
       </c>
       <c r="J48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>